<commit_message>
Preparing for SAMM v1.5 release.
</commit_message>
<xml_diff>
--- a/v1.5/Release Candidate/OpenSAMM_Assessment_Toolbox_v1.5_RC1.xlsx
+++ b/v1.5/Release Candidate/OpenSAMM_Assessment_Toolbox_v1.5_RC1.xlsx
@@ -32177,10 +32177,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y134"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="B56" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="topRight" activeCell="W1" sqref="W1:X1048576"/>
+      <selection pane="topRight" activeCell="W109" sqref="W109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -39092,7 +39092,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G109" formula="1"/>
+    <ignoredError sqref="G109 K109 O109 S109 W109" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>